<commit_message>
done autotest, correst cases & strategy
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>№1</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Ввести в поля блока "Стоимость" значения от: 2000000, до: 5000000</t>
   </si>
   <si>
-    <t xml:space="preserve">При вводе появлялись подсказки вводимых значений, после ввода значений в каждое поле, количество предложений или уменьшалось или оставалось прежним</t>
+    <t xml:space="preserve">При вводе появлялись подсказки вводимых значений, после ввода значений в каждое поле.</t>
   </si>
   <si>
     <t xml:space="preserve">Ввести в поля блока "Площадь" от: 25, до 50</t>
@@ -74,16 +74,19 @@
     <t xml:space="preserve">В блоке "Район" выбрать "Центр: Дом печати"</t>
   </si>
   <si>
-    <t xml:space="preserve">При нажатии на кнопку "Выбрать" появлось всплывающее окно, у выбранного значения проставилась отметка в чекбоксе, количество предложений или уменьшалось или оставалось прежним</t>
+    <t xml:space="preserve">При нажатии на кнопку "Выбрать" появилось всплывающее окно, у выбранного значения проставилась отметка в чекбоксе.</t>
   </si>
   <si>
     <t xml:space="preserve">В блоке "Улица" выбрать "Максима Горького"</t>
   </si>
   <si>
+    <t xml:space="preserve">При нажатии на кнопку "Выбрать" появился выпадающий список , у выбранного значения проставилась отметка в чекбоксе.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Нажать на кнопку "Показать N предложений"*</t>
   </si>
   <si>
-    <t xml:space="preserve">Осуществлён переход на страницу с результатами поиска</t>
+    <t xml:space="preserve">Осуществлён переход к результам поиска</t>
   </si>
   <si>
     <t xml:space="preserve">*N - количественное значение, рассчитанное системой</t>
@@ -152,7 +155,7 @@
     <t xml:space="preserve">У выбранного параметра в чекбоксе появилась отметка, в блоке "Тип недвижимости" указано "Выбрано: 1"</t>
   </si>
   <si>
-    <t xml:space="preserve">Ввести в поля блока "Стоимость" значения от: 10, до: 20</t>
+    <t xml:space="preserve">Ввести в поля блока "Площадь кухни" значения от: 10, до: 20</t>
   </si>
   <si>
     <t xml:space="preserve">После ввода значений в каждое поле, количество предложений или уменьшалось или оставалось прежним</t>
@@ -260,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,7 +291,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -297,6 +300,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -897,7 +903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" ht="57">
+    <row r="6" ht="28.5">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -913,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="57">
+    <row r="7" ht="28.5">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -929,36 +935,36 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" ht="71.25">
+    <row r="8" ht="42.75">
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" ht="71.25">
+    <row r="9" ht="42.75">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="6" t="s">
-        <v>19</v>
+      <c r="E9" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" ht="28.5">
@@ -966,21 +972,21 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>22</v>
+      <c r="E10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -1037,10 +1043,10 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1057,7 +1063,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -1102,15 +1108,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="42.75">
@@ -1118,15 +1124,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="57">
@@ -1134,15 +1140,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" ht="42.75">
@@ -1150,21 +1156,21 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" ht="42.75">
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -1207,10 +1213,10 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1272,15 +1278,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" ht="28.5">
@@ -1288,15 +1294,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="57">
@@ -1304,15 +1310,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" ht="28.5">
@@ -1320,31 +1326,31 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="42.75">
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>45</v>
+      <c r="B9" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" ht="42.75">
@@ -1352,15 +1358,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
       <c r="E10" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" ht="42.75">
@@ -1368,15 +1374,15 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
       <c r="E11" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" ht="42.75">
@@ -1384,15 +1390,15 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" ht="28.5">
@@ -1400,21 +1406,21 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>22</v>
+      <c r="E13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" ht="28.5">
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" ht="14.25">

</xml_diff>